<commit_message>
correcciones importación de statements
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/templates/statementImportTemplate.xlsx
+++ b/backend/src/main/resources/templates/statementImportTemplate.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos\OSMOSYS_2023\backend\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DE653F-AA51-407F-B16E-17A1CC22606F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357A60FF-8653-4EF2-9141-60761EF9C966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{717C7CAA-251A-4996-954C-C684B1BD58E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="catalogo_declaraciones" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -663,12 +663,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,53 +679,69 @@
   <dxfs count="17">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -743,25 +762,25 @@
   <autoFilter ref="A1:N49" xr:uid="{22EC3F25-7CEA-4632-BA8E-A57F89B2F429}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{22DCFAA0-BACF-4530-A492-83C9A07A689D}" name="AREA DE IMPACTO CODIGO" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{F3FB7BD1-B7E5-4BE5-A972-C5C394E97C46}" name="AREA DE IMPACTO" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{F3FB7BD1-B7E5-4BE5-A972-C5C394E97C46}" name="AREA DE IMPACTO" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{061FC3F2-137D-4762-9667-440A5AF21EBC}" name="DECLARACION DE IMPACTO CODIGO" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{5A522B2A-3029-40DF-B854-3F9914B805AA}" name="DECLARACION DE IMPACTO" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{40051232-E930-44DE-B476-AE522539AF05}" name="AREA DE EFECTO CODIGO" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{6605E762-2D50-4821-B5F9-6C3AB61AF7FA}" name="AREA DE EFECTO" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{061FC3F2-137D-4762-9667-440A5AF21EBC}" name="DECLARACION DE IMPACTO CODIGO" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{5A522B2A-3029-40DF-B854-3F9914B805AA}" name="DECLARACION DE IMPACTO" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{40051232-E930-44DE-B476-AE522539AF05}" name="AREA DE EFECTO CODIGO" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{6605E762-2D50-4821-B5F9-6C3AB61AF7FA}" name="AREA DE EFECTO" dataDxfId="12">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EDC81B0C-321C-47BE-981F-E43529631002}" name="DECLARACION DE EFECTO CODIGO" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{901422DA-CABE-434B-8CB9-9FCDBE46E03B}" name="DECLARACION DE EFECTO" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{48E6A62D-5026-4F14-8197-DE0FCBE3E796}" name="DECLARACION DE PRODUCTO CODIGO" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{2323959F-E8A9-4848-98F9-39BB72C00FB4}" name="DECLARACION DE PRODUCTO" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{611D2709-A304-481F-8E73-9594985D414E}" name="PILAR CODIGO" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{68A118F0-FE9D-4683-9981-4A5BA0C6D06C}" name="PILAR" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{EDC81B0C-321C-47BE-981F-E43529631002}" name="DECLARACION DE EFECTO CODIGO" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{901422DA-CABE-434B-8CB9-9FCDBE46E03B}" name="DECLARACION DE EFECTO" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{48E6A62D-5026-4F14-8197-DE0FCBE3E796}" name="DECLARACION DE PRODUCTO CODIGO" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{2323959F-E8A9-4848-98F9-39BB72C00FB4}" name="DECLARACION DE PRODUCTO" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{611D2709-A304-481F-8E73-9594985D414E}" name="PILAR CODIGO" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{68A118F0-FE9D-4683-9981-4A5BA0C6D06C}" name="PILAR" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{DBF0B12D-9D2E-4A88-AA3B-3B7945386F92}" name="SITUACION CODIGO" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{3DDD8815-FD95-4B90-B0F7-3F107BC1F0BE}" name="SITUACION" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{DBF0B12D-9D2E-4A88-AA3B-3B7945386F92}" name="SITUACION CODIGO" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{3DDD8815-FD95-4B90-B0F7-3F107BC1F0BE}" name="SITUACION" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -795,7 +814,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BDCE93F0-4C66-4090-9AFA-356201DAE9AF}" name="Pillars" displayName="Pillars" ref="G1:H5" totalsRowShown="0">
   <autoFilter ref="G1:H5" xr:uid="{BDCE93F0-4C66-4090-9AFA-356201DAE9AF}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{65CDFF3F-645E-4460-9940-A61CF89755B5}" name="code" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{65CDFF3F-645E-4460-9940-A61CF89755B5}" name="code" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{90800186-949D-45C2-93FE-8A47EC277A51}" name="description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1113,7 +1132,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1136,2349 +1155,2349 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="str">
+      <c r="F2" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Acceso al territorio, registro y documentación</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="1" t="str">
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="str">
+      <c r="B3" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="str">
+      <c r="F3" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Acceso al territorio, registro y documentación</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="1" t="str">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="str">
+      <c r="B4" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="str">
+      <c r="F4" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Acceso al territorio, registro y documentación</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="1" t="str">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="str">
+      <c r="B5" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="str">
+      <c r="F5" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Determinación de la condición</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" s="1" t="str">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="str">
+      <c r="B6" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="str">
+      <c r="F6" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Determinación de la condición</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="1" t="str">
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="str">
+      <c r="B7" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="str">
+      <c r="F7" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Determinación de la condición</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="1" t="str">
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="str">
+      <c r="B8" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="1" t="str">
+      <c r="F8" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Seguridad y acceso a la justicia</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" s="1" t="str">
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="156.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="str">
+      <c r="B9" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="str">
+      <c r="F9" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Seguridad y acceso a la justicia</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="1" t="str">
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="str">
+      <c r="B10" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="1" t="str">
+      <c r="F10" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N10" s="1" t="str">
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="str">
+      <c r="B11" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="1" t="str">
+      <c r="F11" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="1" t="str">
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="str">
+      <c r="B12" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="1" t="str">
+      <c r="F12" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="1" t="str">
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="str">
+      <c r="B13" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="1" t="str">
+      <c r="F13" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Violencia sexual y de género</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="1" t="str">
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="str">
+      <c r="B14" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="1" t="str">
+      <c r="F14" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Violencia sexual y de género</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N14" s="1" t="str">
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="str">
+      <c r="B15" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="1" t="str">
+      <c r="F15" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Violencia sexual y de género</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="1">
-        <v>1</v>
-      </c>
-      <c r="L15" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N15" s="1" t="str">
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="str">
+      <c r="B16" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="1" t="str">
+      <c r="F16" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Violencia sexual y de género</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="1">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" s="1" t="str">
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="str">
+      <c r="B17" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="1" t="str">
+      <c r="F17" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Protección de la infancia</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="1">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N17" s="1" t="str">
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="str">
+      <c r="B18" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="1" t="str">
+      <c r="F18" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Protección de la infancia</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N18" s="1" t="str">
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1" t="str">
+      <c r="B19" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Logro de entornos de protección favorables</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="1" t="str">
+      <c r="F19" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Protección de la infancia</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K19" s="1">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N19" s="1" t="str">
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="1" t="str">
+      <c r="B20" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="1" t="str">
+      <c r="F20" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Educación</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="1">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N20" s="1" t="str">
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="1" t="str">
+      <c r="B21" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="1" t="str">
+      <c r="F21" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Educación</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K21" s="1">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N21" s="1" t="str">
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1" t="str">
+      <c r="B22" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="1" t="str">
+      <c r="F22" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Educación</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K22" s="1">
-        <v>1</v>
-      </c>
-      <c r="L22" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N22" s="1" t="str">
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
+      <c r="L22" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="1" t="str">
+      <c r="B23" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="1" t="str">
+      <c r="F23" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Educación</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="1">
-        <v>1</v>
-      </c>
-      <c r="L23" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N23" s="1" t="str">
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="1" t="str">
+      <c r="B24" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="1" t="str">
+      <c r="F24" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Agua limpia, saneamiento e higiene</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="K24" s="1">
-        <v>1</v>
-      </c>
-      <c r="L24" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N24" s="1" t="str">
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="1" t="str">
+      <c r="B25" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="1" t="str">
+      <c r="F25" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Agua limpia, saneamiento e higiene</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K25" s="1">
-        <v>1</v>
-      </c>
-      <c r="L25" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N25" s="1" t="str">
+      <c r="K25" s="3">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="1" t="str">
+      <c r="B26" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="1" t="str">
+      <c r="F26" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Agua limpia, saneamiento e higiene</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K26" s="1">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N26" s="1" t="str">
+      <c r="K26" s="3">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N26" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="1" t="str">
+      <c r="B27" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="1" t="str">
+      <c r="F27" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K27" s="1">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N27" s="1" t="str">
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N27" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="1" t="str">
+      <c r="B28" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F28" s="1" t="str">
+      <c r="F28" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N28" s="1" t="str">
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="1" t="str">
+      <c r="B29" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="1" t="str">
+      <c r="F29" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K29" s="1">
-        <v>1</v>
-      </c>
-      <c r="L29" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N29" s="1" t="str">
+      <c r="K29" s="3">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="1" t="str">
+      <c r="B30" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="1" t="str">
+      <c r="F30" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K30" s="1">
-        <v>1</v>
-      </c>
-      <c r="L30" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N30" s="1" t="str">
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N30" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="1" t="str">
+      <c r="B31" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="1" t="str">
+      <c r="F31" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I31" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K31" s="1">
-        <v>1</v>
-      </c>
-      <c r="L31" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N31" s="1" t="str">
+      <c r="K31" s="3">
+        <v>1</v>
+      </c>
+      <c r="L31" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N31" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="1" t="str">
+      <c r="B32" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="1" t="str">
+      <c r="F32" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I32" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J32" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="K32" s="1">
-        <v>1</v>
-      </c>
-      <c r="L32" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N32" s="1" t="str">
+      <c r="K32" s="3">
+        <v>1</v>
+      </c>
+      <c r="L32" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="1" t="str">
+      <c r="B33" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Haciendo realidad el ejercicio de los derechos en entornos seguros</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="1" t="str">
+      <c r="F33" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Bienestar y necesidades básicas</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I33" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J33" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="K33" s="1">
-        <v>1</v>
-      </c>
-      <c r="L33" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N33" s="1" t="str">
+      <c r="K33" s="3">
+        <v>1</v>
+      </c>
+      <c r="L33" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="1" t="str">
+      <c r="B34" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F34" s="1" t="str">
+      <c r="F34" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Reasentamiento y vías complementarias</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I34" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="J34" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="K34" s="1">
-        <v>1</v>
-      </c>
-      <c r="L34" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N34" s="1" t="str">
+      <c r="K34" s="3">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N34" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="1" t="str">
+      <c r="B35" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F35" s="1" t="str">
+      <c r="F35" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Reasentamiento y vías complementarias</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K35" s="1">
-        <v>1</v>
-      </c>
-      <c r="L35" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N35" s="1" t="str">
+      <c r="K35" s="3">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="1" t="str">
+      <c r="B36" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F36" s="1" t="str">
+      <c r="F36" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Autosuficiencia, inclusión económica y medios de vida</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K36" s="1">
-        <v>1</v>
-      </c>
-      <c r="L36" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N36" s="1" t="str">
+      <c r="K36" s="3">
+        <v>1</v>
+      </c>
+      <c r="L36" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N36" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B37" s="1" t="str">
+      <c r="B37" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F37" s="1" t="str">
+      <c r="F37" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Autosuficiencia, inclusión económica y medios de vida</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I37" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="K37" s="1">
-        <v>1</v>
-      </c>
-      <c r="L37" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N37" s="1" t="str">
+      <c r="K37" s="3">
+        <v>1</v>
+      </c>
+      <c r="L37" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N37" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="1" t="str">
+      <c r="B38" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F38" s="1" t="str">
+      <c r="F38" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Autosuficiencia, inclusión económica y medios de vida</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I38" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J38" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
-      <c r="L38" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N38" s="1" t="str">
+      <c r="K38" s="3">
+        <v>1</v>
+      </c>
+      <c r="L38" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N38" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="1" t="str">
+      <c r="B39" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F39" s="1" t="str">
+      <c r="F39" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Autosuficiencia, inclusión económica y medios de vida</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I39" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J39" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="K39" s="1">
-        <v>1</v>
-      </c>
-      <c r="L39" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N39" s="1" t="str">
+      <c r="K39" s="3">
+        <v>1</v>
+      </c>
+      <c r="L39" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N39" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="1" t="str">
+      <c r="B40" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="1" t="str">
+      <c r="F40" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I40" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="K40" s="1">
-        <v>1</v>
-      </c>
-      <c r="L40" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N40" s="1" t="str">
+      <c r="K40" s="3">
+        <v>1</v>
+      </c>
+      <c r="L40" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="1" t="str">
+      <c r="B41" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="1" t="str">
+      <c r="F41" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I41" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J41" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K41" s="1">
-        <v>1</v>
-      </c>
-      <c r="L41" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N41" s="1" t="str">
+      <c r="K41" s="3">
+        <v>1</v>
+      </c>
+      <c r="L41" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N41" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="1" t="str">
+      <c r="B42" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="1" t="str">
+      <c r="F42" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I42" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K42" s="1">
-        <v>1</v>
-      </c>
-      <c r="L42" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N42" s="1" t="str">
+      <c r="K42" s="3">
+        <v>1</v>
+      </c>
+      <c r="L42" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N42" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="1" t="str">
+      <c r="B43" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F43" s="1" t="str">
+      <c r="F43" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Participación comunitaria y empoderamiento de la mujer</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I43" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K43" s="1">
-        <v>1</v>
-      </c>
-      <c r="L43" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N43" s="1" t="str">
+      <c r="K43" s="3">
+        <v>1</v>
+      </c>
+      <c r="L43" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N43" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B44" s="1" t="str">
+      <c r="B44" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F44" s="1" t="str">
+      <c r="F44" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Participación comunitaria y empoderamiento de la mujer</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I44" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="J44" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="K44" s="1">
-        <v>1</v>
-      </c>
-      <c r="L44" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N44" s="1" t="str">
+      <c r="K44" s="3">
+        <v>1</v>
+      </c>
+      <c r="L44" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N44" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="1" t="str">
+      <c r="B45" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F45" s="1" t="str">
+      <c r="F45" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Participación comunitaria y empoderamiento de la mujer</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I45" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="J45" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K45" s="1">
-        <v>1</v>
-      </c>
-      <c r="L45" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N45" s="1" t="str">
+      <c r="K45" s="3">
+        <v>1</v>
+      </c>
+      <c r="L45" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N45" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="114" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="1" t="str">
+      <c r="B46" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F46" s="1" t="str">
+      <c r="F46" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Participación comunitaria y empoderamiento de la mujer</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G46" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="I46" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="J46" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="K46" s="1">
-        <v>1</v>
-      </c>
-      <c r="L46" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N46" s="1" t="str">
+      <c r="K46" s="3">
+        <v>1</v>
+      </c>
+      <c r="L46" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N46" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B47" s="1" t="str">
+      <c r="B47" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F47" s="1" t="str">
+      <c r="F47" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I47" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="J47" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="K47" s="1">
-        <v>1</v>
-      </c>
-      <c r="L47" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N47" s="1" t="str">
+      <c r="K47" s="3">
+        <v>1</v>
+      </c>
+      <c r="L47" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N47" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B48" s="1" t="str">
+      <c r="B48" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="1" t="str">
+      <c r="F48" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I48" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="J48" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K48" s="1">
-        <v>1</v>
-      </c>
-      <c r="L48" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N48" s="1" t="str">
+      <c r="K48" s="3">
+        <v>1</v>
+      </c>
+      <c r="L48" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N48" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="1" t="str">
+      <c r="B49" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE IMPACTO CODIGO]],AreasImpacto[#All],2,FALSE)</f>
         <v>Empoderamiento de las comunidades y logro de la igualdad de género</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F49" s="1" t="str">
+      <c r="F49" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AREA DE EFECTO CODIGO]],AreasResultado[#All],2,FALSE)</f>
         <v>Integración y otras soluciones locales</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="I49" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="J49" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K49" s="1">
-        <v>1</v>
-      </c>
-      <c r="L49" s="1" t="str">
-        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
-        <v>Programa Global de Refugiados</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N49" s="1" t="str">
+      <c r="K49" s="3">
+        <v>1</v>
+      </c>
+      <c r="L49" s="3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[PILAR CODIGO]],Pillars[],2,FALSE)</f>
+        <v>Programa Global de Refugiados</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N49" s="3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[SITUACION CODIGO]],situations[#All],2,FALSE)</f>
         <v>Protección y Soluciones Mixtas</v>
       </c>
@@ -3495,7 +3514,7 @@
           <x14:formula1>
             <xm:f>Options!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A49 C2:C49</xm:sqref>
+          <xm:sqref>A2:A49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A03A881-E91E-48D3-B6FE-8E28B6557148}">
           <x14:formula1>

</xml_diff>